<commit_message>
Global Argentine reference designators and OOI Barcodes
Added missing OOI barcodes and serial numbers.  Corrected engineering
reference designators, changed CTDMO and PHSEN reference designators to
nominal values.
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GA02HYPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GA02HYPM_00001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\IRAD\IRAD 2015\Programs\OOI Phase 2\Post Delivery 7 support\Asset Management Data\ingestion-csvs_20151204\ingestion-csvs\GA02HYPM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5436" yWindow="7716" windowWidth="26844" windowHeight="10164" activeTab="1"/>
+    <workbookView xWindow="5430" yWindow="7710" windowWidth="26850" windowHeight="10170" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="68">
   <si>
     <t>Ref Des</t>
   </si>
@@ -166,19 +166,7 @@
     <t>GA02HYPM-MFC04-01-ZPLSGA000 unit not deployed</t>
   </si>
   <si>
-    <t>GA02HYPM-WFP02-00-ENG000000</t>
-  </si>
-  <si>
-    <t>GA02HYPM-GP001-00-ENG000000</t>
-  </si>
-  <si>
     <t>GA02HYPM</t>
-  </si>
-  <si>
-    <t>GA02HYPM-WFP03-00-ENG000000</t>
-  </si>
-  <si>
-    <t>GA02HYPM-RIM01-02-CTDMOG046</t>
   </si>
   <si>
     <r>
@@ -273,6 +261,21 @@
   </si>
   <si>
     <t>N00129</t>
+  </si>
+  <si>
+    <t>GA02HYPM-WFP02-00-WFPENG000</t>
+  </si>
+  <si>
+    <t>GA02HYPM-WFP03-00-WFPENG000</t>
+  </si>
+  <si>
+    <t>GA02HYPM-RIM01-00-SIOENG000</t>
+  </si>
+  <si>
+    <t>OL000005</t>
+  </si>
+  <si>
+    <t>GA02HYPM-RIM01-02-CTDMOG039</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1166,7 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1210,7 +1213,6 @@
     <xf numFmtId="165" fontId="14" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1220,7 +1222,6 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1516,7 +1517,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1551,7 +1552,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1766,69 +1767,69 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="13.109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.6640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="17.109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="17.77734375" style="3" customWidth="1"/>
-    <col min="15" max="16384" width="8.77734375" style="3"/>
+    <col min="1" max="1" width="13.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="27" t="s">
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>46</v>
+    <row r="2" spans="1:14" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>44</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>30</v>
@@ -1853,7 +1854,7 @@
         <v>5200</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="12">
@@ -1865,60 +1866,60 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E3" s="13"/>
       <c r="F3" s="14"/>
       <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
-    </row>
-    <row r="5" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="22"/>
-    </row>
-    <row r="6" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
-    </row>
-    <row r="7" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-    </row>
-    <row r="8" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
-    </row>
-    <row r="9" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="22"/>
-    </row>
-    <row r="10" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+    </row>
+    <row r="5" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+    </row>
+    <row r="6" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+    </row>
+    <row r="7" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+    </row>
+    <row r="8" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+    </row>
+    <row r="9" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+    </row>
+    <row r="10" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E10" s="13"/>
       <c r="F10" s="14"/>
       <c r="G10" s="13"/>
     </row>
-    <row r="11" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E11" s="13"/>
       <c r="F11" s="14"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E12" s="13"/>
       <c r="F12" s="14"/>
       <c r="G12" s="13"/>
     </row>
-    <row r="13" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
       <c r="G13" s="13"/>
     </row>
-    <row r="14" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E14" s="13"/>
       <c r="F14" s="14"/>
       <c r="G14" s="13"/>
     </row>
-    <row r="15" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
       <c r="G15" s="13"/>
     </row>
-    <row r="16" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E16" s="13"/>
       <c r="F16" s="14"/>
       <c r="G16" s="13"/>
@@ -1938,60 +1939,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="78.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.77734375" style="1"/>
+    <col min="8" max="8" width="26.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="78.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="26" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:9" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="26" t="s">
+      <c r="B1" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="26" t="s">
+      <c r="E1" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>52</v>
+      <c r="B3" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>30</v>
@@ -1999,8 +2000,8 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" s="22" t="s">
-        <v>66</v>
+      <c r="E3" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="F3" s="1">
         <v>3279</v>
@@ -2015,12 +2016,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>52</v>
+      <c r="B4" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
@@ -2028,8 +2029,8 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>66</v>
+      <c r="E4" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="F4" s="1">
         <v>3279</v>
@@ -2041,12 +2042,12 @@
         <v>1.7379999999999999E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>52</v>
+      <c r="B5" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>30</v>
@@ -2054,8 +2055,8 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>66</v>
+      <c r="E5" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="F5" s="1">
         <v>3279</v>
@@ -2067,12 +2068,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>52</v>
+      <c r="B6" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>30</v>
@@ -2080,8 +2081,8 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>66</v>
+      <c r="E6" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="F6" s="1">
         <v>3279</v>
@@ -2093,12 +2094,12 @@
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>52</v>
+      <c r="B7" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>30</v>
@@ -2106,8 +2107,8 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" s="22" t="s">
-        <v>66</v>
+      <c r="E7" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="F7" s="1">
         <v>3279</v>
@@ -2122,12 +2123,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>52</v>
+      <c r="B8" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>30</v>
@@ -2135,8 +2136,8 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="22" t="s">
-        <v>66</v>
+      <c r="E8" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="F8" s="1">
         <v>3279</v>
@@ -2151,12 +2152,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>52</v>
+      <c r="B9" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>30</v>
@@ -2164,8 +2165,8 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="22" t="s">
-        <v>66</v>
+      <c r="E9" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="F9" s="1">
         <v>3279</v>
@@ -2173,19 +2174,19 @@
       <c r="G9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="23">
         <v>1.0960000000000001</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>52</v>
+      <c r="B10" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>30</v>
@@ -2193,8 +2194,8 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>66</v>
+      <c r="E10" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="F10" s="1">
         <v>3279</v>
@@ -2209,12 +2210,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>52</v>
+      <c r="B12" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>30</v>
@@ -2222,8 +2223,8 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E12" s="22" t="s">
-        <v>65</v>
+      <c r="E12" s="20" t="s">
+        <v>61</v>
       </c>
       <c r="F12" s="1">
         <v>1473</v>
@@ -2238,12 +2239,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>52</v>
+      <c r="B13" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>30</v>
@@ -2251,8 +2252,8 @@
       <c r="D13" s="1">
         <v>1</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>65</v>
+      <c r="E13" s="20" t="s">
+        <v>61</v>
       </c>
       <c r="F13" s="1">
         <v>1473</v>
@@ -2264,12 +2265,12 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>52</v>
+      <c r="B15" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>30</v>
@@ -2277,8 +2278,8 @@
       <c r="D15" s="1">
         <v>1</v>
       </c>
-      <c r="E15" s="22" t="s">
-        <v>64</v>
+      <c r="E15" s="20" t="s">
+        <v>60</v>
       </c>
       <c r="F15" s="1">
         <v>135</v>
@@ -2290,12 +2291,12 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>52</v>
+      <c r="B16" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>30</v>
@@ -2303,8 +2304,8 @@
       <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>64</v>
+      <c r="E16" s="20" t="s">
+        <v>60</v>
       </c>
       <c r="F16" s="1">
         <v>135</v>
@@ -2316,12 +2317,12 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="22" t="s">
-        <v>52</v>
+      <c r="B18" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>30</v>
@@ -2329,8 +2330,8 @@
       <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="E18" s="22" t="s">
-        <v>63</v>
+      <c r="E18" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="F18" s="1">
         <v>1110</v>
@@ -2342,12 +2343,12 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>52</v>
+      <c r="B19" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>30</v>
@@ -2355,8 +2356,8 @@
       <c r="D19" s="1">
         <v>1</v>
       </c>
-      <c r="E19" s="22" t="s">
-        <v>63</v>
+      <c r="E19" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="F19" s="1">
         <v>1110</v>
@@ -2368,12 +2369,12 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>52</v>
+      <c r="B21" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>30</v>
@@ -2381,8 +2382,8 @@
       <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="22" t="s">
-        <v>62</v>
+      <c r="E21" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="F21" s="1">
         <v>3278</v>
@@ -2397,12 +2398,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="22" t="s">
-        <v>52</v>
+      <c r="B22" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>30</v>
@@ -2410,8 +2411,8 @@
       <c r="D22" s="1">
         <v>1</v>
       </c>
-      <c r="E22" s="22" t="s">
-        <v>62</v>
+      <c r="E22" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="F22" s="1">
         <v>3278</v>
@@ -2423,12 +2424,12 @@
         <v>1.702E-6</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="22" t="s">
-        <v>52</v>
+      <c r="B23" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>30</v>
@@ -2436,8 +2437,8 @@
       <c r="D23" s="1">
         <v>1</v>
       </c>
-      <c r="E23" s="22" t="s">
-        <v>62</v>
+      <c r="E23" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="F23" s="1">
         <v>3278</v>
@@ -2449,12 +2450,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="22" t="s">
-        <v>52</v>
+      <c r="B24" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>30</v>
@@ -2462,8 +2463,8 @@
       <c r="D24" s="1">
         <v>1</v>
       </c>
-      <c r="E24" s="22" t="s">
-        <v>62</v>
+      <c r="E24" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="F24" s="1">
         <v>3278</v>
@@ -2475,12 +2476,12 @@
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="22" t="s">
-        <v>52</v>
+      <c r="B25" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>30</v>
@@ -2488,8 +2489,8 @@
       <c r="D25" s="1">
         <v>1</v>
       </c>
-      <c r="E25" s="22" t="s">
-        <v>62</v>
+      <c r="E25" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="F25" s="1">
         <v>3278</v>
@@ -2504,12 +2505,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="22" t="s">
-        <v>52</v>
+      <c r="B26" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>30</v>
@@ -2517,8 +2518,8 @@
       <c r="D26" s="1">
         <v>1</v>
       </c>
-      <c r="E26" s="22" t="s">
-        <v>62</v>
+      <c r="E26" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="F26" s="1">
         <v>3278</v>
@@ -2533,12 +2534,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="22" t="s">
-        <v>52</v>
+      <c r="B27" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>30</v>
@@ -2546,8 +2547,8 @@
       <c r="D27" s="1">
         <v>1</v>
       </c>
-      <c r="E27" s="22" t="s">
-        <v>62</v>
+      <c r="E27" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="F27" s="1">
         <v>3278</v>
@@ -2562,12 +2563,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="22" t="s">
-        <v>52</v>
+      <c r="B28" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>30</v>
@@ -2575,8 +2576,8 @@
       <c r="D28" s="1">
         <v>1</v>
       </c>
-      <c r="E28" s="22" t="s">
-        <v>62</v>
+      <c r="E28" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="F28" s="1">
         <v>3278</v>
@@ -2591,12 +2592,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="22" t="s">
-        <v>52</v>
+      <c r="B30" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>30</v>
@@ -2604,8 +2605,8 @@
       <c r="D30" s="1">
         <v>1</v>
       </c>
-      <c r="E30" s="22" t="s">
-        <v>61</v>
+      <c r="E30" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="F30" s="1">
         <v>1475</v>
@@ -2617,12 +2618,12 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="22" t="s">
-        <v>52</v>
+      <c r="B31" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>30</v>
@@ -2630,8 +2631,8 @@
       <c r="D31" s="1">
         <v>1</v>
       </c>
-      <c r="E31" s="22" t="s">
-        <v>61</v>
+      <c r="E31" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="F31" s="1">
         <v>1475</v>
@@ -2643,12 +2644,12 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="22" t="s">
-        <v>52</v>
+      <c r="B33" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>30</v>
@@ -2656,8 +2657,8 @@
       <c r="D33" s="1">
         <v>1</v>
       </c>
-      <c r="E33" s="22" t="s">
-        <v>60</v>
+      <c r="E33" s="20" t="s">
+        <v>56</v>
       </c>
       <c r="F33" s="1">
         <v>129</v>
@@ -2669,12 +2670,12 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="22" t="s">
-        <v>52</v>
+      <c r="B34" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>30</v>
@@ -2682,8 +2683,8 @@
       <c r="D34" s="1">
         <v>1</v>
       </c>
-      <c r="E34" s="22" t="s">
-        <v>60</v>
+      <c r="E34" s="20" t="s">
+        <v>56</v>
       </c>
       <c r="F34" s="1">
         <v>129</v>
@@ -2695,12 +2696,12 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="22" t="s">
-        <v>52</v>
+      <c r="B36" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>30</v>
@@ -2708,8 +2709,8 @@
       <c r="D36" s="1">
         <v>1</v>
       </c>
-      <c r="E36" s="22" t="s">
-        <v>59</v>
+      <c r="E36" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="F36" s="1">
         <v>1117</v>
@@ -2721,12 +2722,12 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="22" t="s">
-        <v>52</v>
+      <c r="B37" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>30</v>
@@ -2734,8 +2735,8 @@
       <c r="D37" s="1">
         <v>1</v>
       </c>
-      <c r="E37" s="22" t="s">
-        <v>59</v>
+      <c r="E37" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="F37" s="1">
         <v>1117</v>
@@ -2747,17 +2748,17 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I39" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>52</v>
+    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>30</v>
@@ -2765,26 +2766,26 @@
       <c r="D41" s="1">
         <v>1</v>
       </c>
-      <c r="E41" s="22" t="s">
-        <v>57</v>
+      <c r="E41" s="20" t="s">
+        <v>53</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H41" s="24">
+      <c r="H41" s="22">
         <v>1450</v>
       </c>
-      <c r="I41" s="18"/>
-    </row>
-    <row r="42" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B42" s="22" t="s">
-        <v>52</v>
+      <c r="I41" s="17"/>
+    </row>
+    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>30</v>
@@ -2792,11 +2793,11 @@
       <c r="D42" s="1">
         <v>1</v>
       </c>
-      <c r="E42" s="22" t="s">
-        <v>57</v>
+      <c r="E42" s="20" t="s">
+        <v>53</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>6</v>
@@ -2804,14 +2805,14 @@
       <c r="H42" s="1">
         <v>-42.981666666666669</v>
       </c>
-      <c r="I42" s="18"/>
-    </row>
-    <row r="43" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A43" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>52</v>
+      <c r="I42" s="17"/>
+    </row>
+    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>30</v>
@@ -2819,11 +2820,11 @@
       <c r="D43" s="1">
         <v>1</v>
       </c>
-      <c r="E43" s="22" t="s">
-        <v>57</v>
+      <c r="E43" s="20" t="s">
+        <v>53</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>7</v>
@@ -2831,69 +2832,72 @@
       <c r="H43" s="1">
         <v>-42.4985</v>
       </c>
-      <c r="I43" s="18"/>
-    </row>
-    <row r="45" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="22" t="s">
+      <c r="I43" s="17"/>
+    </row>
+    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F45" s="21">
+        <v>13994</v>
+      </c>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="17"/>
+    </row>
+    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I46" s="17"/>
+    </row>
+    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1</v>
-      </c>
-      <c r="F45" s="23">
-        <v>13994</v>
-      </c>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="18"/>
-    </row>
-    <row r="46" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" s="1">
-        <v>1</v>
-      </c>
-      <c r="E46" s="22" t="s">
+      <c r="F47" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="F46" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="I46" s="18"/>
-    </row>
-    <row r="47" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
-      <c r="E47" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="F47" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="I47" s="18"/>
+      <c r="I47" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Corrected ref desig, added OOI Barcodes, created integration sheets
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GA02HYPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GA02HYPM_00001.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="7710" windowWidth="26850" windowHeight="10170" activeTab="1"/>
+    <workbookView xWindow="5430" yWindow="7710" windowWidth="26850" windowHeight="10170"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -1763,8 +1763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="G25" sqref="G24:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1843,7 +1843,9 @@
       <c r="F2" s="11">
         <v>0.79166666666666663</v>
       </c>
-      <c r="G2" s="15"/>
+      <c r="G2" s="15">
+        <v>42323</v>
+      </c>
       <c r="H2" s="10" t="s">
         <v>41</v>
       </c>
@@ -1939,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updates to Argentine Basin CTDMO calibration coefficients
The following calibration coefficients added to all Argentine Basin
CTDMOs per
Redmine ticket 10208. Updates made by Rebecca Travis.

CC_wbotc
CC_a0
CC_a1
CC_a2
CC_a3
CC_ptempa0
CC_ptempa1
CC_ptempa2
CC_ptca0
CC_ptca1
CC_ptca2
CC_ptcb0
CC_ptcb1
CC_ptcb2
CC_pa0
CC_pa1
CC_pa2
CC_g
CC_h
CC_i
CC_j
CC_cpcor
CC_ctcor
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GA02HYPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GA02HYPM_00001.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rtravis\Desktop\Cal Sheet project\GA cal sheets RT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10160" yWindow="1560" windowWidth="26860" windowHeight="10180" activeTab="1"/>
+    <workbookView xWindow="10164" yWindow="1560" windowWidth="26856" windowHeight="10176" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -17,7 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="93">
   <si>
     <t>Ref Des</t>
   </si>
@@ -188,28 +193,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>37-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>12406</t>
-    </r>
-  </si>
-  <si>
     <t>Mooring OOIBARCODE</t>
   </si>
   <si>
@@ -271,19 +254,98 @@
   </si>
   <si>
     <t>GA02HYPM-RIM01-02-CTDMOG039</t>
+  </si>
+  <si>
+    <t>Induction ID</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>CC_wbotc</t>
+  </si>
+  <si>
+    <t>CC_a0</t>
+  </si>
+  <si>
+    <t>CC_a1</t>
+  </si>
+  <si>
+    <t>CC_a2</t>
+  </si>
+  <si>
+    <t>CC_a3</t>
+  </si>
+  <si>
+    <t>CC_ptempa0</t>
+  </si>
+  <si>
+    <t>CC_ptempa1</t>
+  </si>
+  <si>
+    <t>CC_ptempa2</t>
+  </si>
+  <si>
+    <t>CC_ptca0</t>
+  </si>
+  <si>
+    <t>CC_ptca1</t>
+  </si>
+  <si>
+    <t>CC_ptca2</t>
+  </si>
+  <si>
+    <t>CC_ptcb0</t>
+  </si>
+  <si>
+    <t>CC_ptcb1</t>
+  </si>
+  <si>
+    <t>CC_ptcb2</t>
+  </si>
+  <si>
+    <t>CC_pa0</t>
+  </si>
+  <si>
+    <t>CC_pa1</t>
+  </si>
+  <si>
+    <t>CC_pa2</t>
+  </si>
+  <si>
+    <t>CC_g</t>
+  </si>
+  <si>
+    <t>CC_h</t>
+  </si>
+  <si>
+    <t>CC_i</t>
+  </si>
+  <si>
+    <t>CC_j</t>
+  </si>
+  <si>
+    <t>CC_cpcor</t>
+  </si>
+  <si>
+    <t>CC_ctcor</t>
+  </si>
+  <si>
+    <t>37-12406</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="48" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -597,8 +659,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFBFBFBF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -800,6 +875,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1161,7 +1242,7 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1236,6 +1317,36 @@
     </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="37" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="14" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="47" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="199">
@@ -1453,7 +1564,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1762,28 +1873,28 @@
       <selection activeCell="G25" sqref="G24:G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.6640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="17.1640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" style="3" customWidth="1"/>
     <col min="14" max="14" width="17.6640625" style="3" customWidth="1"/>
     <col min="15" max="16384" width="8.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" ht="28">
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>0</v>
@@ -1819,9 +1930,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1">
+    <row r="2" spans="1:14" s="8" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>44</v>
@@ -1863,60 +1974,60 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="8" customFormat="1">
+    <row r="3" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E3" s="13"/>
       <c r="F3" s="14"/>
       <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="1:14" customFormat="1">
+    <row r="4" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
     </row>
-    <row r="5" spans="1:14" customFormat="1">
+    <row r="5" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
     </row>
-    <row r="6" spans="1:14" customFormat="1">
+    <row r="6" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
     </row>
-    <row r="7" spans="1:14" customFormat="1">
+    <row r="7" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
     </row>
-    <row r="8" spans="1:14" customFormat="1">
+    <row r="8" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="20"/>
     </row>
-    <row r="9" spans="1:14" customFormat="1">
+    <row r="9" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
     </row>
-    <row r="10" spans="1:14" s="8" customFormat="1">
+    <row r="10" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E10" s="13"/>
       <c r="F10" s="14"/>
       <c r="G10" s="13"/>
     </row>
-    <row r="11" spans="1:14" s="8" customFormat="1">
+    <row r="11" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E11" s="13"/>
       <c r="F11" s="14"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="12" spans="1:14" s="8" customFormat="1">
+    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E12" s="13"/>
       <c r="F12" s="14"/>
       <c r="G12" s="13"/>
     </row>
-    <row r="13" spans="1:14" s="8" customFormat="1">
+    <row r="13" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
       <c r="G13" s="13"/>
     </row>
-    <row r="14" spans="1:14" s="8" customFormat="1">
+    <row r="14" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E14" s="13"/>
       <c r="F14" s="14"/>
       <c r="G14" s="13"/>
     </row>
-    <row r="15" spans="1:14" s="8" customFormat="1">
+    <row r="15" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
       <c r="G15" s="13"/>
     </row>
-    <row r="16" spans="1:14" s="8" customFormat="1">
+    <row r="16" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E16" s="13"/>
       <c r="F16" s="14"/>
       <c r="G16" s="13"/>
@@ -1934,32 +2045,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="78.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="24" customFormat="1" ht="28">
+    <row r="1" spans="1:9" s="24" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>1</v>
@@ -1968,7 +2079,7 @@
         <v>24</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F1" s="24" t="s">
         <v>2</v>
@@ -1983,13 +2094,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1"/>
-    <row r="3" spans="1:9">
+    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>30</v>
@@ -1998,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F3" s="1">
         <v>3279</v>
@@ -2013,12 +2124,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
@@ -2027,7 +2138,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="1">
         <v>3279</v>
@@ -2039,12 +2150,12 @@
         <v>1.7379999999999999E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>30</v>
@@ -2053,7 +2164,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F5" s="1">
         <v>3279</v>
@@ -2065,12 +2176,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>30</v>
@@ -2079,7 +2190,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F6" s="1">
         <v>3279</v>
@@ -2091,12 +2202,12 @@
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>30</v>
@@ -2105,7 +2216,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F7" s="1">
         <v>3279</v>
@@ -2120,12 +2231,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>30</v>
@@ -2134,7 +2245,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F8" s="1">
         <v>3279</v>
@@ -2149,12 +2260,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>30</v>
@@ -2163,7 +2274,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F9" s="1">
         <v>3279</v>
@@ -2178,12 +2289,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>30</v>
@@ -2192,7 +2303,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F10" s="1">
         <v>3279</v>
@@ -2207,12 +2318,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>30</v>
@@ -2221,7 +2332,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" s="1">
         <v>1473</v>
@@ -2236,12 +2347,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>30</v>
@@ -2250,7 +2361,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13" s="1">
         <v>1473</v>
@@ -2262,12 +2373,12 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>30</v>
@@ -2276,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F15" s="1">
         <v>135</v>
@@ -2288,12 +2399,12 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>30</v>
@@ -2302,7 +2413,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F16" s="1">
         <v>135</v>
@@ -2314,12 +2425,12 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>30</v>
@@ -2328,7 +2439,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" s="1">
         <v>1110</v>
@@ -2340,12 +2451,12 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>30</v>
@@ -2354,7 +2465,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F19" s="1">
         <v>1110</v>
@@ -2366,12 +2477,12 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>30</v>
@@ -2380,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F21" s="1">
         <v>3278</v>
@@ -2395,12 +2506,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>30</v>
@@ -2409,7 +2520,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F22" s="1">
         <v>3278</v>
@@ -2421,12 +2532,12 @@
         <v>1.702E-6</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>30</v>
@@ -2435,7 +2546,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F23" s="1">
         <v>3278</v>
@@ -2447,12 +2558,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>30</v>
@@ -2461,7 +2572,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F24" s="1">
         <v>3278</v>
@@ -2473,12 +2584,12 @@
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>30</v>
@@ -2487,7 +2598,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F25" s="1">
         <v>3278</v>
@@ -2502,12 +2613,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>30</v>
@@ -2516,7 +2627,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F26" s="1">
         <v>3278</v>
@@ -2531,12 +2642,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>30</v>
@@ -2545,7 +2656,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F27" s="1">
         <v>3278</v>
@@ -2560,12 +2671,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>30</v>
@@ -2574,7 +2685,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F28" s="1">
         <v>3278</v>
@@ -2589,12 +2700,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>30</v>
@@ -2603,7 +2714,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F30" s="1">
         <v>1475</v>
@@ -2615,12 +2726,12 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>30</v>
@@ -2629,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F31" s="1">
         <v>1475</v>
@@ -2641,12 +2752,12 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>30</v>
@@ -2655,7 +2766,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33" s="1">
         <v>129</v>
@@ -2667,12 +2778,12 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>30</v>
@@ -2681,7 +2792,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F34" s="1">
         <v>129</v>
@@ -2693,12 +2804,12 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>30</v>
@@ -2707,7 +2818,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F36" s="1">
         <v>1117</v>
@@ -2719,12 +2830,12 @@
         <v>-42.981666666666669</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>30</v>
@@ -2733,7 +2844,7 @@
         <v>1</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F37" s="1">
         <v>1117</v>
@@ -2745,156 +2856,813 @@
         <v>-42.4985</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I39" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="G41" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41" s="1">
-        <v>1</v>
-      </c>
-      <c r="E41" s="20" t="s">
+      <c r="H41" s="28">
+        <v>46</v>
+      </c>
+      <c r="I41" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="J41" s="29">
+        <v>163</v>
+      </c>
+      <c r="M41" s="22"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="34">
+        <v>1</v>
+      </c>
+      <c r="E42" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G42" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="30">
+        <v>-42.981666666666669</v>
+      </c>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="34">
+        <v>1</v>
+      </c>
+      <c r="E43" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F43" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G43" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" s="30">
+        <v>-42.4985</v>
+      </c>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="34">
+        <v>1</v>
+      </c>
+      <c r="E44" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G44" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="H44" s="28">
+        <v>1450</v>
+      </c>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="34">
+        <v>1</v>
+      </c>
+      <c r="E45" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F45" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G45" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="H45" s="35">
+        <v>2.9704000000000002E-7</v>
+      </c>
+      <c r="I45" s="32"/>
+    </row>
+    <row r="46" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="34">
+        <v>1</v>
+      </c>
+      <c r="E46" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G46" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="H46" s="36">
+        <v>-1.7791730000000001E-4</v>
+      </c>
+      <c r="I46" s="33"/>
+    </row>
+    <row r="47" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="34">
+        <v>1</v>
+      </c>
+      <c r="E47" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G47" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="H47" s="36">
+        <v>3.2352709999999997E-4</v>
+      </c>
+      <c r="I47" s="33"/>
+    </row>
+    <row r="48" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="34">
+        <v>1</v>
+      </c>
+      <c r="E48" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F48" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G48" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H48" s="36">
+        <v>-5.7633569999999996E-6</v>
+      </c>
+      <c r="I48" s="33"/>
+    </row>
+    <row r="49" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A49" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="34">
+        <v>1</v>
+      </c>
+      <c r="E49" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F49" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G49" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="H49" s="36">
+        <v>2.3730599999999999E-7</v>
+      </c>
+      <c r="I49" s="33"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="34">
+        <v>1</v>
+      </c>
+      <c r="E50" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G50" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H50" s="35">
+        <v>-68.4649</v>
+      </c>
+      <c r="I50" s="33"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="34">
+        <v>1</v>
+      </c>
+      <c r="E51" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F51" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G51" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H51" s="35">
+        <v>5.2325360000000001E-2</v>
+      </c>
+      <c r="I51" s="33"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="34">
+        <v>1</v>
+      </c>
+      <c r="E52" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F52" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G52" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="H52" s="35">
+        <v>-6.1446659999999997E-7</v>
+      </c>
+      <c r="I52" s="33"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="34">
+        <v>1</v>
+      </c>
+      <c r="E53" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F53" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H53" s="35">
+        <v>524777.1</v>
+      </c>
+      <c r="I53" s="33"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" s="34">
+        <v>1</v>
+      </c>
+      <c r="E54" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F54" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G54" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H54" s="35">
+        <v>4.06996</v>
+      </c>
+      <c r="I54" s="33"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="34">
+        <v>1</v>
+      </c>
+      <c r="E55" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F55" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G55" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="H55" s="35">
+        <v>-5.0070370000000003E-2</v>
+      </c>
+      <c r="I55" s="33"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" s="34">
+        <v>1</v>
+      </c>
+      <c r="E56" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F56" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G56" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H56" s="35">
+        <v>25.333749999999998</v>
+      </c>
+      <c r="I56" s="33"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C57" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" s="34">
+        <v>1</v>
+      </c>
+      <c r="E57" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F57" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G57" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="H57" s="35">
+        <v>3.5E-4</v>
+      </c>
+      <c r="I57" s="33"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D58" s="34">
+        <v>1</v>
+      </c>
+      <c r="E58" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F58" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G58" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="H58" s="35">
+        <v>0</v>
+      </c>
+      <c r="I58" s="33"/>
+    </row>
+    <row r="59" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A59" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C59" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D59" s="34">
+        <v>1</v>
+      </c>
+      <c r="E59" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F59" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G59" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="H59" s="36">
+        <v>0.30505320000000002</v>
+      </c>
+      <c r="I59" s="33"/>
+    </row>
+    <row r="60" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A60" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C60" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" s="34">
+        <v>1</v>
+      </c>
+      <c r="E60" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F60" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G60" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="H60" s="36">
+        <v>4.6217699999999999E-3</v>
+      </c>
+      <c r="I60" s="33"/>
+    </row>
+    <row r="61" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A61" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D61" s="34">
+        <v>1</v>
+      </c>
+      <c r="E61" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F61" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G61" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="H61" s="36">
+        <v>-1.265751E-11</v>
+      </c>
+      <c r="I61" s="33"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C62" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D62" s="34">
+        <v>1</v>
+      </c>
+      <c r="E62" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F62" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G62" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="H62" s="35">
+        <v>-0.97570259999999998</v>
+      </c>
+      <c r="I62" s="33"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C63" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" s="34">
+        <v>1</v>
+      </c>
+      <c r="E63" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F63" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G63" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="H63" s="35">
+        <v>0.1531312</v>
+      </c>
+      <c r="I63" s="33"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C64" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D64" s="34">
+        <v>1</v>
+      </c>
+      <c r="E64" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F64" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G64" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H64" s="35">
+        <v>-1.05344E-4</v>
+      </c>
+      <c r="I64" s="33"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C65" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D65" s="34">
+        <v>1</v>
+      </c>
+      <c r="E65" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F65" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G65" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="H65" s="35">
+        <v>3.1230060000000002E-5</v>
+      </c>
+      <c r="I65" s="33"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66" s="34">
+        <v>1</v>
+      </c>
+      <c r="E66" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F66" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G66" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="H66" s="35">
+        <v>-9.5700000000000003E-8</v>
+      </c>
+      <c r="I66" s="33"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C67" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D67" s="34">
+        <v>1</v>
+      </c>
+      <c r="E67" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F67" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G67" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="H67" s="35">
+        <v>3.2499999999999998E-6</v>
+      </c>
+      <c r="I67" s="33"/>
+    </row>
+    <row r="69" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A69" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B69" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D69" s="1">
+        <v>1</v>
+      </c>
+      <c r="E69" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F69" s="21">
+        <v>13994</v>
+      </c>
+      <c r="G69" s="16"/>
+      <c r="H69" s="16"/>
+      <c r="I69" s="17"/>
+    </row>
+    <row r="70" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A70" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B70" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D70" s="1">
+        <v>1</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F70" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="I70" s="17"/>
+    </row>
+    <row r="71" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A71" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D71" s="1">
+        <v>1</v>
+      </c>
+      <c r="E71" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F71" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H41" s="22">
-        <v>1450</v>
-      </c>
-      <c r="I41" s="17"/>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D42" s="1">
-        <v>1</v>
-      </c>
-      <c r="E42" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H42" s="1">
-        <v>-42.981666666666669</v>
-      </c>
-      <c r="I42" s="17"/>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43" s="1">
-        <v>1</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H43" s="1">
-        <v>-42.4985</v>
-      </c>
-      <c r="I43" s="17"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F45" s="21">
-        <v>13994</v>
-      </c>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="17"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" s="1">
-        <v>1</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F46" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="I46" s="17"/>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="B47" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
-      <c r="E47" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F47" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="I47" s="17"/>
+      <c r="I71" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>